<commit_message>
Added Attendance Marking Feature
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -1,52 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Check-In</t>
-  </si>
-  <si>
-    <t>Check-Out</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -54,26 +48,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -120,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -152,10 +215,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,7 +249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -363,27 +424,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Check-In</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Check-Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Harshit Saraswat</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>44513.82614364583</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>44513.83074774306</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Harshit Saraswat</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>44513.83076476852</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>44513.83080909722</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Harshit Saraswat</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>44513.83081765047</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>44513.83084804398</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Harshit Saraswat</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>44513.83127752315</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>44513.8313628125</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Harshit Saraswat</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>44513.83187018075</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>